<commit_message>
trabajando en el deploy
</commit_message>
<xml_diff>
--- a/server/LISTAS/ma/BANQUETA ESCALERA Y TAPIZADA DISMAY.xlsx
+++ b/server/LISTAS/ma/BANQUETA ESCALERA Y TAPIZADA DISMAY.xlsx
@@ -908,7 +908,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="27" t="n">
-        <v>45289</v>
+        <v>45302</v>
       </c>
       <c r="E1" s="4" t="n"/>
     </row>
@@ -1079,18 +1079,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:D11"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="A12:D12"/>
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B35:C35"/>
     <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="B28:C28"/>
     <mergeCell ref="A9:D9"/>
+    <mergeCell ref="B36:C36"/>
     <mergeCell ref="B29:C29"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="A10:D10"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="A32:D32"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>

<commit_message>
corregiendo errores y mejorando en el step 2
</commit_message>
<xml_diff>
--- a/server/LISTAS/ma/BANQUETA ESCALERA Y TAPIZADA DISMAY.xlsx
+++ b/server/LISTAS/ma/BANQUETA ESCALERA Y TAPIZADA DISMAY.xlsx
@@ -908,7 +908,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="27" t="n">
-        <v>45302</v>
+        <v>45306</v>
       </c>
       <c r="E1" s="4" t="n"/>
     </row>
@@ -1079,18 +1079,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="A12:D12"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="A11:D11"/>
     <mergeCell ref="A10:D10"/>
-    <mergeCell ref="A11:D11"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="A12:D12"/>
-    <mergeCell ref="A1:D1"/>
     <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B30:C30"/>
     <mergeCell ref="A32:D32"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B29:C29"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="portrait" paperSize="9" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>